<commit_message>
Updated Excel Functions, Driver engine
</commit_message>
<xml_diff>
--- a/HybridKeywordDrivenFramework/src/Resource/KeywordDrivenTest.xlsx
+++ b/HybridKeywordDrivenFramework/src/Resource/KeywordDrivenTest.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajak/eclipse-workspace-2020/HybridKeywordDrivenFramework/src/Resource/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajak/git/selenium/HybridKeywordDrivenFramework/src/Resource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DB4430-5D48-4C49-8931-3E1B0B6F97DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE0BE5E-EF74-B444-86BB-5367FCEEFD9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14420" activeTab="1" xr2:uid="{C7DDD537-EF73-5345-91CC-5BA3217DB98C}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="4" r:id="rId1"/>
-    <sheet name="TestStepsModel1" sheetId="1" r:id="rId2"/>
-    <sheet name="TestStepsModel2" sheetId="5" r:id="rId3"/>
-    <sheet name="TestStepModel3" sheetId="6" r:id="rId4"/>
-    <sheet name="Advanced1" sheetId="3" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
+    <sheet name="TestSuite" sheetId="7" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="4" r:id="rId2"/>
+    <sheet name="TestStepsModel1" sheetId="1" r:id="rId3"/>
+    <sheet name="TestStepsModel2" sheetId="5" r:id="rId4"/>
+    <sheet name="TestStepModel3" sheetId="6" r:id="rId5"/>
+    <sheet name="Advanced1" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="167">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -240,9 +241,6 @@
   </si>
   <si>
     <t>TestData</t>
-  </si>
-  <si>
-    <t>RunMode</t>
   </si>
   <si>
     <t>PlatformSignUp_02</t>
@@ -752,6 +750,81 @@
   </si>
   <si>
     <t>closeButton</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>TestStepDescriptions</t>
+  </si>
+  <si>
+    <t>TestCaseDescription</t>
+  </si>
+  <si>
+    <t>TestCaseSheetName</t>
+  </si>
+  <si>
+    <t>TestStepsModel2</t>
+  </si>
+  <si>
+    <t>TestStepsModel1</t>
+  </si>
+  <si>
+    <t>TestStepsModel3</t>
+  </si>
+  <si>
+    <t>TestSuiteID</t>
+  </si>
+  <si>
+    <t>SAPAIPlatform</t>
+  </si>
+  <si>
+    <t>TestSuiteDescription</t>
+  </si>
+  <si>
+    <t>TestSuiteExecution</t>
+  </si>
+  <si>
+    <t>Suite 1</t>
+  </si>
+  <si>
+    <t>Suite 2</t>
+  </si>
+  <si>
+    <t>API Suite</t>
+  </si>
+  <si>
+    <t>Regression Suite</t>
+  </si>
+  <si>
+    <t>API Test 1</t>
+  </si>
+  <si>
+    <t>Regression Test 1</t>
+  </si>
+  <si>
+    <t>Regression Test Case</t>
+  </si>
+  <si>
+    <t>API Test Case</t>
+  </si>
+  <si>
+    <t>Sheet X</t>
+  </si>
+  <si>
+    <t>Sheet Y</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>yyy</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -820,7 +893,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -830,6 +903,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,13 +938,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1168,61 +1262,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAAB3CC-5A35-D643-94F1-8667356C3E63}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945442EE-285F-6D44-BE0A-81F80B2901DA}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAAB3CC-5A35-D643-94F1-8667356C3E63}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
+      <c r="D4" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1231,12 +1499,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E85920D-5D15-3349-9223-D0E633C23D10}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,16 +1554,16 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1312,13 +1580,13 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1332,16 +1600,16 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1355,16 +1623,16 @@
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1378,16 +1646,16 @@
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1401,16 +1669,16 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" t="s">
         <v>78</v>
-      </c>
-      <c r="F7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1424,16 +1692,16 @@
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1447,16 +1715,16 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1470,16 +1738,16 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1493,16 +1761,16 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1516,16 +1784,16 @@
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1539,16 +1807,16 @@
         <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1562,16 +1830,16 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1585,16 +1853,16 @@
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1608,16 +1876,16 @@
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1631,16 +1899,16 @@
         <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1657,13 +1925,13 @@
         <v>57</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1677,12 +1945,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C613074-865D-2B4A-88BC-F2B63F4EDBFE}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1703,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1732,16 +2000,16 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1758,13 +2026,13 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1781,13 +2049,13 @@
         <v>55</v>
       </c>
       <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1804,13 +2072,13 @@
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1824,16 +2092,16 @@
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1847,16 +2115,16 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1870,16 +2138,16 @@
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1893,16 +2161,16 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1916,16 +2184,16 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1939,16 +2207,16 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1965,13 +2233,13 @@
         <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1988,13 +2256,13 @@
         <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2005,19 +2273,19 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2034,13 +2302,13 @@
         <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2054,16 +2322,16 @@
         <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" t="s">
-        <v>101</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2077,16 +2345,16 @@
         <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2103,13 +2371,13 @@
         <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2117,7 +2385,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
@@ -2126,13 +2394,105 @@
         <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22">
+        <v>123</v>
+      </c>
+      <c r="F22" t="s">
+        <v>163</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F23" t="s">
+        <v>164</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2142,12 +2502,14 @@
     <hyperlink ref="G9" r:id="rId2" xr:uid="{47F357CB-4919-EB45-8443-37CC6EB1A440}"/>
     <hyperlink ref="G3" r:id="rId3" xr:uid="{4AF15459-C4B4-6A45-AECC-C657D70A7273}"/>
     <hyperlink ref="G11" r:id="rId4" xr:uid="{391DD6FD-576C-AF40-ACE1-23A22B63709B}"/>
+    <hyperlink ref="G21" r:id="rId5" xr:uid="{992BCBA5-D789-1D41-999D-F8D6AE2DE6A6}"/>
+    <hyperlink ref="G23" r:id="rId6" xr:uid="{BD65F3FB-AB54-714A-8458-079E421E7685}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A0C033-6694-EA46-9DC0-C5962F05330F}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -2182,7 +2544,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>69</v>
@@ -2202,16 +2564,16 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2228,13 +2590,13 @@
         <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2251,13 +2613,13 @@
         <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2274,13 +2636,13 @@
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2294,16 +2656,16 @@
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2317,16 +2679,16 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2340,16 +2702,16 @@
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2363,16 +2725,16 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2386,16 +2748,16 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2409,16 +2771,16 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2435,13 +2797,13 @@
         <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -2458,13 +2820,13 @@
         <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -2475,19 +2837,19 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2504,13 +2866,13 @@
         <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -2524,16 +2886,16 @@
         <v>35</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
         <v>100</v>
       </c>
-      <c r="E16" t="s">
-        <v>101</v>
-      </c>
       <c r="F16" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2547,16 +2909,16 @@
         <v>36</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -2573,13 +2935,13 @@
         <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -2587,7 +2949,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
@@ -2596,13 +2958,13 @@
         <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2616,7 +2978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B961A4-ABDF-BB44-8E76-C5CAF4E0DE3C}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -2899,7 +3261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C8B831-F2CE-354E-B2FF-622359132597}">
   <dimension ref="A1:A20"/>
   <sheetViews>

</xml_diff>